<commit_message>
Week 1 tasks created
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -559,7 +559,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-09-14 17:01</t>
+          <t>2025-09-14 18:42</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -595,7 +595,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>FastAPI</t>
+          <t>Learn FastAPI</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-09-14 17:01</t>
+          <t>2025-09-14 18:42</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>learn Subprocess library in python</t>
+          <t>Learn Subprocess</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-09-14 17:02</t>
+          <t>2025-09-14 18:42</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">

</xml_diff>